<commit_message>
Removes unneeded data columns from JSON array
</commit_message>
<xml_diff>
--- a/Testing-Files/Height_0_20198281030_QTOF_small_missing_data.xlsx
+++ b/Testing-Files/Height_0_20198281030_QTOF_small_missing_data.xlsx
@@ -565,7 +565,7 @@
   <dimension ref="A1:DB4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1533,9 +1533,6 @@
       <c r="B4" s="1" t="n">
         <v>6.397</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>268.10495</v>
-      </c>
       <c r="D4" s="1" t="s">
         <v>119</v>
       </c>

</xml_diff>